<commit_message>
Add Tank mounting rail excel file
</commit_message>
<xml_diff>
--- a/OpsAndMats/8025043-1.xlsx
+++ b/OpsAndMats/8025043-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="112">
   <si>
     <t>Item</t>
   </si>
@@ -146,88 +146,64 @@
     <t>Variable Overhead Cost</t>
   </si>
   <si>
+    <t>8025043-1</t>
+  </si>
+  <si>
+    <t>Drive Unit Stop Assembly</t>
+  </si>
+  <si>
+    <t>ASY010</t>
+  </si>
+  <si>
+    <t>Assembly, System</t>
+  </si>
+  <si>
+    <t>6680001</t>
+  </si>
+  <si>
+    <t>6230007-1</t>
+  </si>
+  <si>
+    <t>2033501</t>
+  </si>
+  <si>
+    <t>3031003</t>
+  </si>
+  <si>
+    <t>2577401</t>
+  </si>
+  <si>
+    <t>2402812</t>
+  </si>
+  <si>
+    <t>8025044-1</t>
+  </si>
+  <si>
     <t>8025042</t>
   </si>
   <si>
-    <t>8025043-1</t>
+    <t>1/2", crutch tip, black</t>
+  </si>
+  <si>
+    <t>shaft collar, steel, 1/2"</t>
+  </si>
+  <si>
+    <t>Hex Nut, full, ½-13, Pl. Stl.</t>
+  </si>
+  <si>
+    <t>3/8", bevel washer</t>
+  </si>
+  <si>
+    <t>Washer, Split Lock, Med, 3/8, Pl. Stl.</t>
+  </si>
+  <si>
+    <t>HHCS, 3/8-16, 1 1/2, Pl. Stl.</t>
+  </si>
+  <si>
+    <t>Zinc Plated Threaded Rod</t>
   </si>
   <si>
     <t>Support-Drive Unit Stop</t>
-  </si>
-  <si>
-    <t>Drive Unit Stop Assembly</t>
-  </si>
-  <si>
-    <t>ASY010</t>
-  </si>
-  <si>
-    <t>EXT010</t>
-  </si>
-  <si>
-    <t>Assembly, System</t>
-  </si>
-  <si>
-    <t>External Operations</t>
-  </si>
-  <si>
-    <t>8025042-A</t>
-  </si>
-  <si>
-    <t>9816011</t>
-  </si>
-  <si>
-    <t>3110004</t>
-  </si>
-  <si>
-    <t>6680001</t>
-  </si>
-  <si>
-    <t>6230007-1</t>
-  </si>
-  <si>
-    <t>2033501</t>
-  </si>
-  <si>
-    <t>3031003</t>
-  </si>
-  <si>
-    <t>2577401</t>
-  </si>
-  <si>
-    <t>2402812</t>
-  </si>
-  <si>
-    <t>8025044-1</t>
-  </si>
-  <si>
-    <t>Support-Drive Unit, Unplated</t>
-  </si>
-  <si>
-    <t>Zinc Plating</t>
-  </si>
-  <si>
-    <t>thd inserts, 1/2-13 self-tap, cad.plt</t>
-  </si>
-  <si>
-    <t>1/2", crutch tip, black</t>
-  </si>
-  <si>
-    <t>shaft collar, steel, 1/2"</t>
-  </si>
-  <si>
-    <t>Hex Nut, full, ½-13, Pl. Stl.</t>
-  </si>
-  <si>
-    <t>3/8", bevel washer</t>
-  </si>
-  <si>
-    <t>Washer, Split Lock, Med, 3/8, Pl. Stl.</t>
-  </si>
-  <si>
-    <t>HHCS, 3/8-16, 1 1/2, Pl. Stl.</t>
-  </si>
-  <si>
-    <t>Zinc Plated Threaded Rod</t>
   </si>
   <si>
     <t>Unit</t>
@@ -732,7 +708,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AQ12"/>
+  <dimension ref="A1:AQ9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -874,22 +850,22 @@
         <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2">
         <v>10</v>
       </c>
       <c r="G2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" t="s">
         <v>47</v>
       </c>
-      <c r="H2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I2" t="s">
-        <v>51</v>
-      </c>
       <c r="J2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -904,13 +880,13 @@
         <v>8</v>
       </c>
       <c r="S2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="T2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="U2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="V2">
         <v>0</v>
@@ -957,28 +933,28 @@
         <v>43</v>
       </c>
       <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
         <v>45</v>
       </c>
-      <c r="E3">
-        <v>20</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" t="s">
         <v>48</v>
       </c>
-      <c r="H3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I3" t="s">
-        <v>52</v>
-      </c>
       <c r="J3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -987,13 +963,13 @@
         <v>8</v>
       </c>
       <c r="S3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="T3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="U3" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="V3">
         <v>0</v>
@@ -1040,28 +1016,28 @@
         <v>43</v>
       </c>
       <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
         <v>45</v>
       </c>
-      <c r="E4">
-        <v>30</v>
-      </c>
-      <c r="G4" t="s">
-        <v>47</v>
-      </c>
       <c r="H4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" t="s">
         <v>49</v>
       </c>
-      <c r="I4" t="s">
-        <v>53</v>
-      </c>
       <c r="J4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -1070,13 +1046,13 @@
         <v>8</v>
       </c>
       <c r="S4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="T4" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="U4" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="V4">
         <v>0</v>
@@ -1120,31 +1096,31 @@
     </row>
     <row r="5" spans="1:43">
       <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
         <v>44</v>
-      </c>
-      <c r="B5" t="s">
-        <v>46</v>
       </c>
       <c r="E5">
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="J5" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="K5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -1156,10 +1132,10 @@
         <v>4</v>
       </c>
       <c r="T5" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="U5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="V5">
         <v>0</v>
@@ -1203,31 +1179,31 @@
     </row>
     <row r="6" spans="1:43">
       <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" t="s">
         <v>44</v>
-      </c>
-      <c r="B6" t="s">
-        <v>46</v>
       </c>
       <c r="E6">
         <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="J6" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="K6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -1239,10 +1215,10 @@
         <v>4</v>
       </c>
       <c r="T6" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="U6" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="V6">
         <v>0</v>
@@ -1286,31 +1262,31 @@
     </row>
     <row r="7" spans="1:43">
       <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
         <v>44</v>
-      </c>
-      <c r="B7" t="s">
-        <v>46</v>
       </c>
       <c r="E7">
         <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="J7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="K7">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L7">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -1322,10 +1298,10 @@
         <v>4</v>
       </c>
       <c r="T7" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="U7" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="V7">
         <v>0</v>
@@ -1369,31 +1345,31 @@
     </row>
     <row r="8" spans="1:43">
       <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
         <v>44</v>
-      </c>
-      <c r="B8" t="s">
-        <v>46</v>
       </c>
       <c r="E8">
         <v>10</v>
       </c>
       <c r="G8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="J8" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="K8">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="L8">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -1405,10 +1381,10 @@
         <v>4</v>
       </c>
       <c r="T8" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="U8" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="V8">
         <v>0</v>
@@ -1452,31 +1428,31 @@
     </row>
     <row r="9" spans="1:43">
       <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
         <v>44</v>
-      </c>
-      <c r="B9" t="s">
-        <v>46</v>
       </c>
       <c r="E9">
         <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I9" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="J9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="K9">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="L9">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M9">
         <v>0</v>
@@ -1488,10 +1464,10 @@
         <v>4</v>
       </c>
       <c r="T9" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="U9" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="V9">
         <v>0</v>
@@ -1530,255 +1506,6 @@
         <v>0</v>
       </c>
       <c r="AQ9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:43">
-      <c r="A10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10">
-        <v>10</v>
-      </c>
-      <c r="G10" t="s">
-        <v>47</v>
-      </c>
-      <c r="H10" t="s">
-        <v>49</v>
-      </c>
-      <c r="I10" t="s">
-        <v>59</v>
-      </c>
-      <c r="J10" t="s">
-        <v>69</v>
-      </c>
-      <c r="K10">
-        <v>6</v>
-      </c>
-      <c r="L10">
-        <v>6</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="R10" t="s">
-        <v>8</v>
-      </c>
-      <c r="S10">
-        <v>4</v>
-      </c>
-      <c r="T10" t="s">
-        <v>71</v>
-      </c>
-      <c r="U10" t="s">
-        <v>72</v>
-      </c>
-      <c r="V10">
-        <v>0</v>
-      </c>
-      <c r="W10">
-        <v>0</v>
-      </c>
-      <c r="AB10">
-        <v>1</v>
-      </c>
-      <c r="AF10">
-        <v>1</v>
-      </c>
-      <c r="AG10">
-        <v>0</v>
-      </c>
-      <c r="AH10">
-        <v>0</v>
-      </c>
-      <c r="AK10">
-        <v>0</v>
-      </c>
-      <c r="AL10">
-        <v>0</v>
-      </c>
-      <c r="AM10">
-        <v>0</v>
-      </c>
-      <c r="AN10">
-        <v>0</v>
-      </c>
-      <c r="AO10">
-        <v>0</v>
-      </c>
-      <c r="AP10">
-        <v>0</v>
-      </c>
-      <c r="AQ10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:43">
-      <c r="A11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11">
-        <v>10</v>
-      </c>
-      <c r="G11" t="s">
-        <v>47</v>
-      </c>
-      <c r="H11" t="s">
-        <v>49</v>
-      </c>
-      <c r="I11" t="s">
-        <v>60</v>
-      </c>
-      <c r="J11" t="s">
-        <v>70</v>
-      </c>
-      <c r="K11">
-        <v>7</v>
-      </c>
-      <c r="L11">
-        <v>7</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="R11" t="s">
-        <v>8</v>
-      </c>
-      <c r="S11">
-        <v>4</v>
-      </c>
-      <c r="T11" t="s">
-        <v>71</v>
-      </c>
-      <c r="U11" t="s">
-        <v>72</v>
-      </c>
-      <c r="V11">
-        <v>0</v>
-      </c>
-      <c r="W11">
-        <v>0</v>
-      </c>
-      <c r="AB11">
-        <v>1</v>
-      </c>
-      <c r="AF11">
-        <v>1</v>
-      </c>
-      <c r="AG11">
-        <v>0</v>
-      </c>
-      <c r="AH11">
-        <v>0</v>
-      </c>
-      <c r="AK11">
-        <v>0</v>
-      </c>
-      <c r="AL11">
-        <v>0</v>
-      </c>
-      <c r="AM11">
-        <v>0</v>
-      </c>
-      <c r="AN11">
-        <v>0</v>
-      </c>
-      <c r="AO11">
-        <v>0</v>
-      </c>
-      <c r="AP11">
-        <v>0</v>
-      </c>
-      <c r="AQ11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:43">
-      <c r="A12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12">
-        <v>10</v>
-      </c>
-      <c r="G12" t="s">
-        <v>47</v>
-      </c>
-      <c r="H12" t="s">
-        <v>49</v>
-      </c>
-      <c r="I12" t="s">
-        <v>43</v>
-      </c>
-      <c r="J12" t="s">
-        <v>45</v>
-      </c>
-      <c r="K12">
-        <v>8</v>
-      </c>
-      <c r="L12">
-        <v>8</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="R12" t="s">
-        <v>8</v>
-      </c>
-      <c r="S12">
-        <v>4</v>
-      </c>
-      <c r="T12" t="s">
-        <v>71</v>
-      </c>
-      <c r="U12" t="s">
-        <v>72</v>
-      </c>
-      <c r="V12">
-        <v>0</v>
-      </c>
-      <c r="W12">
-        <v>0</v>
-      </c>
-      <c r="AB12">
-        <v>1</v>
-      </c>
-      <c r="AF12">
-        <v>1</v>
-      </c>
-      <c r="AG12">
-        <v>0</v>
-      </c>
-      <c r="AH12">
-        <v>0</v>
-      </c>
-      <c r="AK12">
-        <v>0</v>
-      </c>
-      <c r="AL12">
-        <v>0</v>
-      </c>
-      <c r="AM12">
-        <v>0</v>
-      </c>
-      <c r="AN12">
-        <v>0</v>
-      </c>
-      <c r="AO12">
-        <v>0</v>
-      </c>
-      <c r="AP12">
-        <v>0</v>
-      </c>
-      <c r="AQ12">
         <v>0</v>
       </c>
     </row>
@@ -1789,7 +1516,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AW5"/>
+  <dimension ref="A1:AW2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1821,61 +1548,61 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>23</v>
@@ -1884,64 +1611,64 @@
         <v>24</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="AE1" s="1" t="s">
         <v>27</v>
       </c>
       <c r="AF1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AN1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:49">
@@ -1949,34 +1676,34 @@
         <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2">
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="L2">
         <v>0.5</v>
       </c>
       <c r="M2" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="N2">
         <v>0</v>
       </c>
       <c r="O2" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="P2">
         <v>0.5</v>
@@ -2009,28 +1736,28 @@
         <v>1</v>
       </c>
       <c r="AE2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="AG2" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="AH2" t="s">
         <v>0</v>
       </c>
       <c r="AI2" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="AK2" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="AL2">
         <v>0</v>
       </c>
       <c r="AM2" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="AN2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="AO2">
         <v>0</v>
@@ -2051,336 +1778,6 @@
         <v>0</v>
       </c>
       <c r="AW2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:49">
-      <c r="A3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3">
-        <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="K3" t="s">
-        <v>111</v>
-      </c>
-      <c r="L3">
-        <v>0.5</v>
-      </c>
-      <c r="M3" t="s">
-        <v>112</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3" t="s">
-        <v>113</v>
-      </c>
-      <c r="P3">
-        <v>0.5</v>
-      </c>
-      <c r="R3">
-        <v>100</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>0</v>
-      </c>
-      <c r="V3">
-        <v>0</v>
-      </c>
-      <c r="W3">
-        <v>0</v>
-      </c>
-      <c r="X3">
-        <v>0</v>
-      </c>
-      <c r="Y3">
-        <v>0</v>
-      </c>
-      <c r="AA3">
-        <v>0</v>
-      </c>
-      <c r="AD3">
-        <v>1</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>114</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>115</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>116</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>117</v>
-      </c>
-      <c r="AL3">
-        <v>0</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>118</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>119</v>
-      </c>
-      <c r="AO3">
-        <v>0</v>
-      </c>
-      <c r="AQ3">
-        <v>100</v>
-      </c>
-      <c r="AS3">
-        <v>35</v>
-      </c>
-      <c r="AT3">
-        <v>35</v>
-      </c>
-      <c r="AU3">
-        <v>0</v>
-      </c>
-      <c r="AV3">
-        <v>0</v>
-      </c>
-      <c r="AW3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:49">
-      <c r="A4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4">
-        <v>30</v>
-      </c>
-      <c r="G4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H4" t="s">
-        <v>49</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="K4" t="s">
-        <v>111</v>
-      </c>
-      <c r="L4">
-        <v>0.5</v>
-      </c>
-      <c r="M4" t="s">
-        <v>112</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4" t="s">
-        <v>113</v>
-      </c>
-      <c r="P4">
-        <v>0.5</v>
-      </c>
-      <c r="R4">
-        <v>100</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
-      <c r="Y4">
-        <v>0</v>
-      </c>
-      <c r="AA4">
-        <v>0</v>
-      </c>
-      <c r="AD4">
-        <v>1</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>114</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>115</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>116</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>117</v>
-      </c>
-      <c r="AL4">
-        <v>0</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>118</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>119</v>
-      </c>
-      <c r="AO4">
-        <v>0</v>
-      </c>
-      <c r="AQ4">
-        <v>100</v>
-      </c>
-      <c r="AS4">
-        <v>35</v>
-      </c>
-      <c r="AT4">
-        <v>35</v>
-      </c>
-      <c r="AU4">
-        <v>0</v>
-      </c>
-      <c r="AV4">
-        <v>0</v>
-      </c>
-      <c r="AW4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:49">
-      <c r="A5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5">
-        <v>10</v>
-      </c>
-      <c r="G5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H5" t="s">
-        <v>49</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="K5" t="s">
-        <v>111</v>
-      </c>
-      <c r="L5">
-        <v>0.5</v>
-      </c>
-      <c r="M5" t="s">
-        <v>112</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5" t="s">
-        <v>113</v>
-      </c>
-      <c r="P5">
-        <v>0.5</v>
-      </c>
-      <c r="R5">
-        <v>100</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="V5">
-        <v>0</v>
-      </c>
-      <c r="W5">
-        <v>0</v>
-      </c>
-      <c r="X5">
-        <v>0</v>
-      </c>
-      <c r="Y5">
-        <v>0</v>
-      </c>
-      <c r="AA5">
-        <v>0</v>
-      </c>
-      <c r="AD5">
-        <v>1</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>114</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>115</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>116</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>117</v>
-      </c>
-      <c r="AL5">
-        <v>0</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>118</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>119</v>
-      </c>
-      <c r="AO5">
-        <v>0</v>
-      </c>
-      <c r="AQ5">
-        <v>100</v>
-      </c>
-      <c r="AS5">
-        <v>35</v>
-      </c>
-      <c r="AT5">
-        <v>35</v>
-      </c>
-      <c r="AU5">
-        <v>0</v>
-      </c>
-      <c r="AV5">
-        <v>0</v>
-      </c>
-      <c r="AW5">
         <v>0</v>
       </c>
     </row>

</xml_diff>